<commit_message>
glucose data in spreadsheet
</commit_message>
<xml_diff>
--- a/experiment-data/random-experiments.xlsx
+++ b/experiment-data/random-experiments.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jereeves/git/BiPartGen-Artifact/experiment-data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15BE23B4-CDA6-BD40-A5E9-432559ACE541}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39093CD0-624B-C141-BE58-566FE2790D54}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3900" yWindow="2200" windowWidth="28040" windowHeight="17440" xr2:uid="{F0F9316C-0838-F046-8DA5-10A35F60BEFF}"/>
+    <workbookView xWindow="3900" yWindow="2200" windowWidth="28040" windowHeight="17440" activeTab="4" xr2:uid="{F0F9316C-0838-F046-8DA5-10A35F60BEFF}"/>
   </bookViews>
   <sheets>
     <sheet name="Fig1(Top)" sheetId="1" r:id="rId1"/>
     <sheet name="Fig1(Middle)" sheetId="3" r:id="rId2"/>
     <sheet name="Fig1(Bottom)" sheetId="4" r:id="rId3"/>
     <sheet name="Fig2" sheetId="2" r:id="rId4"/>
+    <sheet name="Glucose and Kissat" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="29">
   <si>
     <t>A Experiments</t>
   </si>
@@ -103,6 +104,27 @@
   </si>
   <si>
     <t>Split-Ord-A</t>
+  </si>
+  <si>
+    <t>Random Graphs</t>
+  </si>
+  <si>
+    <t>Edge = 130</t>
+  </si>
+  <si>
+    <t>Density = 0.98</t>
+  </si>
+  <si>
+    <t>Glucose_4.1</t>
+  </si>
+  <si>
+    <t>phase saving and variable elim disabled</t>
+  </si>
+  <si>
+    <t>Avgs</t>
+  </si>
+  <si>
+    <t>Seed</t>
   </si>
 </sst>
 </file>
@@ -470,7 +492,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B8CACE4-51E2-C741-86FE-7303D742D6BA}">
   <dimension ref="A1:L30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
@@ -1444,7 +1466,7 @@
     <col min="9" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>12</v>
       </c>
@@ -1455,7 +1477,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B2" s="2" t="s">
         <v>1</v>
       </c>
@@ -1487,7 +1509,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B3" s="1">
         <v>1</v>
       </c>
@@ -1519,7 +1541,7 @@
         <v>18.776151833333341</v>
       </c>
     </row>
-    <row r="4" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B4" s="1">
         <v>0.83333299999999999</v>
       </c>
@@ -1551,7 +1573,7 @@
         <v>290.40806500000002</v>
       </c>
     </row>
-    <row r="5" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B5" s="1">
         <v>0.70512799999999998</v>
       </c>
@@ -1583,7 +1605,7 @@
         <v>374.89934333333338</v>
       </c>
     </row>
-    <row r="6" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B6" s="1">
         <v>0.60439600000000004</v>
       </c>
@@ -1615,7 +1637,7 @@
         <v>494.18636499999991</v>
       </c>
     </row>
-    <row r="7" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B7" s="1">
         <v>0.52381</v>
       </c>
@@ -1647,7 +1669,7 @@
         <v>375.25581499999998</v>
       </c>
     </row>
-    <row r="8" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B8" s="1">
         <v>0.45833299999999999</v>
       </c>
@@ -1679,7 +1701,7 @@
         <v>240.98545166666659</v>
       </c>
     </row>
-    <row r="9" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B9" s="1">
         <v>0.40441199999999999</v>
       </c>
@@ -1711,7 +1733,7 @@
         <v>159.59689883333331</v>
       </c>
     </row>
-    <row r="10" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B10" s="1">
         <v>0.35947699999999999</v>
       </c>
@@ -1743,7 +1765,7 @@
         <v>123.6425326666667</v>
       </c>
     </row>
-    <row r="11" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B11" s="1">
         <v>0.32163700000000001</v>
       </c>
@@ -1775,7 +1797,7 @@
         <v>66.549493333333345</v>
       </c>
     </row>
-    <row r="12" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B12" s="1">
         <v>0.28947400000000001</v>
       </c>
@@ -1807,7 +1829,7 @@
         <v>46.317277500000003</v>
       </c>
     </row>
-    <row r="13" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B13" s="1">
         <v>0.261905</v>
       </c>
@@ -1839,7 +1861,7 @@
         <v>27.425988</v>
       </c>
     </row>
-    <row r="14" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B14" s="1">
         <v>0.217391</v>
       </c>
@@ -1871,7 +1893,7 @@
         <v>19.483018000000001</v>
       </c>
     </row>
-    <row r="15" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B15" s="1">
         <v>0.183333</v>
       </c>
@@ -1903,7 +1925,7 @@
         <v>4.8030963500000006</v>
       </c>
     </row>
-    <row r="16" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B16" s="1">
         <v>0.156695</v>
       </c>
@@ -1935,7 +1957,7 @@
         <v>2.1671914166666668</v>
       </c>
     </row>
-    <row r="17" spans="2:12" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B17" s="1">
         <v>0.13546800000000001</v>
       </c>
@@ -1967,7 +1989,7 @@
         <v>1.1561661666666669</v>
       </c>
     </row>
-    <row r="18" spans="2:12" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B18" s="1">
         <v>0.11828</v>
       </c>
@@ -1999,7 +2021,7 @@
         <v>0.46346538333333331</v>
       </c>
     </row>
-    <row r="19" spans="2:12" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B19" s="1">
         <v>0.104167</v>
       </c>
@@ -2031,7 +2053,7 @@
         <v>0.22122263333333339</v>
       </c>
     </row>
-    <row r="20" spans="2:12" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B20" s="1">
         <v>9.2437000000000005E-2</v>
       </c>
@@ -2063,7 +2085,7 @@
         <v>0.1242557666666667</v>
       </c>
     </row>
-    <row r="21" spans="2:12" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B21" s="1">
         <v>8.2583000000000004E-2</v>
       </c>
@@ -2095,7 +2117,7 @@
         <v>9.3211883333333342E-2</v>
       </c>
     </row>
-    <row r="22" spans="2:12" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B22" s="1">
         <v>7.4223999999999998E-2</v>
       </c>
@@ -2127,7 +2149,7 @@
         <v>7.3607699999999984E-2</v>
       </c>
     </row>
-    <row r="23" spans="2:12" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B23" s="1">
         <v>6.7072999999999994E-2</v>
       </c>
@@ -3238,7 +3260,7 @@
     <col min="10" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>14</v>
       </c>
@@ -3249,7 +3271,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B2" s="2" t="s">
         <v>1</v>
       </c>
@@ -3278,7 +3300,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B3" s="1">
         <v>0.81818199999999996</v>
       </c>
@@ -3307,7 +3329,7 @@
         <v>49.524131666666698</v>
       </c>
     </row>
-    <row r="4" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B4" s="1">
         <v>0.68181800000000004</v>
       </c>
@@ -3336,7 +3358,7 @@
         <v>52.575433333333329</v>
       </c>
     </row>
-    <row r="5" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B5" s="1">
         <v>0.57692299999999996</v>
       </c>
@@ -3365,7 +3387,7 @@
         <v>68.025006666666656</v>
       </c>
     </row>
-    <row r="6" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B6" s="1">
         <v>0.49450499999999997</v>
       </c>
@@ -3394,7 +3416,7 @@
         <v>93.084415000000035</v>
       </c>
     </row>
-    <row r="7" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B7" s="1">
         <v>0.42857099999999998</v>
       </c>
@@ -3423,7 +3445,7 @@
         <v>143.24525499999999</v>
       </c>
     </row>
-    <row r="8" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B8" s="1">
         <v>0.375</v>
       </c>
@@ -3452,7 +3474,7 @@
         <v>241.75613333333331</v>
       </c>
     </row>
-    <row r="9" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B9" s="1">
         <v>0.33088200000000001</v>
       </c>
@@ -3481,7 +3503,7 @@
         <v>353.88457333333309</v>
       </c>
     </row>
-    <row r="10" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B10" s="1">
         <v>0.29411799999999999</v>
       </c>
@@ -3510,7 +3532,7 @@
         <v>706.63161666666667</v>
       </c>
     </row>
-    <row r="11" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B11" s="1">
         <v>0.263158</v>
       </c>
@@ -3539,7 +3561,7 @@
         <v>833.41835000000003</v>
       </c>
     </row>
-    <row r="12" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B12" s="1">
         <v>0.236842</v>
       </c>
@@ -3568,7 +3590,7 @@
         <v>1341.120266666667</v>
       </c>
     </row>
-    <row r="13" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B13" s="1">
         <v>0.214286</v>
       </c>
@@ -3597,7 +3619,7 @@
         <v>1592.478666666666</v>
       </c>
     </row>
-    <row r="14" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B14" s="1">
         <v>0.177866</v>
       </c>
@@ -3626,7 +3648,7 @@
         <v>1724.948583333334</v>
       </c>
     </row>
-    <row r="15" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B15" s="1">
         <v>0.15</v>
       </c>
@@ -3655,7 +3677,7 @@
         <v>1710.33915</v>
       </c>
     </row>
-    <row r="16" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B16" s="1">
         <v>0.12820500000000001</v>
       </c>
@@ -3684,7 +3706,7 @@
         <v>1756.586866666667</v>
       </c>
     </row>
-    <row r="17" spans="2:11" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B17" s="1">
         <v>0.110837</v>
       </c>
@@ -3713,7 +3735,7 @@
         <v>1749.492316666667</v>
       </c>
     </row>
-    <row r="18" spans="2:11" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B18" s="1">
         <v>9.6773999999999999E-2</v>
       </c>
@@ -3742,7 +3764,7 @@
         <v>1781.5056500000001</v>
       </c>
     </row>
-    <row r="19" spans="2:11" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B19" s="1">
         <v>8.5226999999999997E-2</v>
       </c>
@@ -3771,7 +3793,7 @@
         <v>1759.6415500000001</v>
       </c>
     </row>
-    <row r="20" spans="2:11" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B20" s="1">
         <v>7.5630000000000003E-2</v>
       </c>
@@ -3800,7 +3822,7 @@
         <v>1757.4112500000001</v>
       </c>
     </row>
-    <row r="21" spans="2:11" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B21" s="1">
         <v>6.7568000000000003E-2</v>
       </c>
@@ -3829,7 +3851,7 @@
         <v>1689.97615</v>
       </c>
     </row>
-    <row r="22" spans="2:11" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B22" s="1">
         <v>6.0728999999999998E-2</v>
       </c>
@@ -3858,7 +3880,7 @@
         <v>1704.2954</v>
       </c>
     </row>
-    <row r="23" spans="2:11" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B23" s="1">
         <v>5.4878000000000003E-2</v>
       </c>
@@ -3887,7 +3909,7 @@
         <v>1748.5218166666671</v>
       </c>
     </row>
-    <row r="24" spans="2:11" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:11" x14ac:dyDescent="0.2">
       <c r="H24" s="1">
         <v>0.117647</v>
       </c>
@@ -3901,7 +3923,7 @@
         <v>1707.0943</v>
       </c>
     </row>
-    <row r="25" spans="2:11" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:11" x14ac:dyDescent="0.2">
       <c r="H25" s="1">
         <v>0.111111</v>
       </c>
@@ -3915,7 +3937,7 @@
         <v>1715.6352999999999</v>
       </c>
     </row>
-    <row r="26" spans="2:11" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:11" x14ac:dyDescent="0.2">
       <c r="H26" s="1">
         <v>0.105105</v>
       </c>
@@ -3929,7 +3951,7 @@
         <v>1659.097935</v>
       </c>
     </row>
-    <row r="27" spans="2:11" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:11" x14ac:dyDescent="0.2">
       <c r="H27" s="1">
         <v>9.9572999999999995E-2</v>
       </c>
@@ -3943,7 +3965,7 @@
         <v>1604.3464316666671</v>
       </c>
     </row>
-    <row r="28" spans="2:11" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:11" x14ac:dyDescent="0.2">
       <c r="H28" s="1">
         <v>9.4466999999999995E-2</v>
       </c>
@@ -3957,7 +3979,7 @@
         <v>1434.1814649999999</v>
       </c>
     </row>
-    <row r="29" spans="2:11" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:11" x14ac:dyDescent="0.2">
       <c r="H29" s="1">
         <v>8.5365999999999997E-2</v>
       </c>
@@ -3971,7 +3993,7 @@
         <v>1492.913741666667</v>
       </c>
     </row>
-    <row r="30" spans="2:11" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:11" x14ac:dyDescent="0.2">
       <c r="H30" s="1">
         <v>7.7519000000000005E-2</v>
       </c>
@@ -3985,7 +4007,7 @@
         <v>1000.394038333333</v>
       </c>
     </row>
-    <row r="31" spans="2:11" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:11" x14ac:dyDescent="0.2">
       <c r="H31" s="1">
         <v>7.0707000000000006E-2</v>
       </c>
@@ -3999,7 +4021,7 @@
         <v>818.09384833333331</v>
       </c>
     </row>
-    <row r="32" spans="2:11" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:11" x14ac:dyDescent="0.2">
       <c r="H32" s="1">
         <v>6.4754999999999993E-2</v>
       </c>
@@ -4013,7 +4035,7 @@
         <v>363.18364500000013</v>
       </c>
     </row>
-    <row r="33" spans="8:11" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="8:11" x14ac:dyDescent="0.2">
       <c r="H33" s="1">
         <v>5.9524000000000001E-2</v>
       </c>
@@ -4025,6 +4047,169 @@
       </c>
       <c r="K33" s="2">
         <v>344.03274016666649</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3204DD6D-39BE-C24C-B277-6D262968219D}">
+  <dimension ref="B2:E13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E26" sqref="E26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="34.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>72.061999999999998</v>
+      </c>
+      <c r="E3">
+        <v>9.51783</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4">
+        <v>2</v>
+      </c>
+      <c r="D4">
+        <v>83.790899999999993</v>
+      </c>
+      <c r="E4">
+        <v>13.6424</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5">
+        <v>3</v>
+      </c>
+      <c r="D5">
+        <v>107.56699999999999</v>
+      </c>
+      <c r="E5">
+        <v>11.6511</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C6">
+        <v>4</v>
+      </c>
+      <c r="D6">
+        <v>91.574399999999997</v>
+      </c>
+      <c r="E6">
+        <v>18.528099999999998</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C7">
+        <v>5</v>
+      </c>
+      <c r="D7">
+        <v>233.376</v>
+      </c>
+      <c r="E7">
+        <v>17.4116</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C8">
+        <v>6</v>
+      </c>
+      <c r="D8">
+        <v>80.226100000000002</v>
+      </c>
+      <c r="E8">
+        <v>10.9032</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C9">
+        <v>7</v>
+      </c>
+      <c r="D9">
+        <v>78.078599999999994</v>
+      </c>
+      <c r="E9">
+        <v>8.7835800000000006</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C10">
+        <v>8</v>
+      </c>
+      <c r="D10">
+        <v>92.423500000000004</v>
+      </c>
+      <c r="E10">
+        <v>10.2142</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C11">
+        <v>9</v>
+      </c>
+      <c r="D11">
+        <v>134.364</v>
+      </c>
+      <c r="E11">
+        <v>8.8500700000000005</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C12">
+        <v>10</v>
+      </c>
+      <c r="D12">
+        <v>110.367</v>
+      </c>
+      <c r="E12">
+        <v>13.7926</v>
+      </c>
+    </row>
+    <row r="13" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C13" t="s">
+        <v>27</v>
+      </c>
+      <c r="D13">
+        <v>108.38294999999999</v>
+      </c>
+      <c r="E13">
+        <v>12.329468</v>
       </c>
     </row>
   </sheetData>

</xml_diff>